<commit_message>
bug fix (multi input from file and sheet logic)
</commit_message>
<xml_diff>
--- a/TestProject/TestProject/wwwroot/upload/template_test.xlsx
+++ b/TestProject/TestProject/wwwroot/upload/template_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/GraduationAssessment/GraduationAssesment/TestProject/TestProject/wwwroot/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5339BFD-DEA8-1845-BDCA-F39A5C90CFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1B68A4-07A6-8642-AF31-BD752316866B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="31240" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="전체질문목록" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="165">
   <si>
     <t>입력하려는 졸업기준의 학과(전공)명을 선택하세요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -312,10 +312,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(예시) 심화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[공통교양] Sheet에 입력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -356,82 +352,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(예시) 컴퓨터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 신입학생</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 2015</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 2017</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 21</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 21</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 36</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 140</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 3.52</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[타학과전공인정] Sheet에 입력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -484,14 +404,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(예시) 6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(예시) 9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>설계학점</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -528,130 +440,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RGC1002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RGC1003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자아와명상1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자아와명상2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나의삶나의비전</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ABC1001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ABC1002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ABC1003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ABC1004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기본소양1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기본소양2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기본소양3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기본소양4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRI4011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRI4012</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PRI4013</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>공학수학2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공학수학3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRI2011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRI2012</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRI2013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물리실험1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>화학실험1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>생물실험1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRI5555</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRI5556</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>생물학개론</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRI0010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRI0011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로그래밍기초와실습</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인터넷프로그래밍</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>개설년도</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -663,6 +455,246 @@
   </si>
   <si>
     <t>OX</t>
+  </si>
+  <si>
+    <t>심화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신입학생</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터공학전공 전산학불인정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16학점 이상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자아와 명상1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자아와 명상2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불교와 인간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기술보고서 작성 및 발표</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EAS1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EAS2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRI4040</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRI4041</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRI4043</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRI4048</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EGC7026</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기술창조와 특허</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기술과 사회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공학경제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공학법제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지속가능한 발전과 인간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미적분학 및 연습 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>확률 및 통계학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이산수학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>창의적공학설계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자료구조와실습</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터구성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시스템소프트웨어와실습</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRI4001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRI4027</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRI4002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRI4003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRI4004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 물리학 및 실험 I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 화학 및 실험 I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 생물학 및 실험 I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 물리학 및 실험 II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 화학 및 실험 II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 생물학 및 실험 II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRI4015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRI4014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGC0017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGC0018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나의삶, 나의비전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGC0003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGC0005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGC1033</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGC1034</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSE2016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSE2017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSE2018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSE2013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSE4074</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSE4067</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터공학종합설계2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터공학종합설계1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSE4066</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공개SW프로젝트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -758,7 +790,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -805,13 +837,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -885,6 +930,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1212,22 +1266,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="2" max="2" width="8.83203125" style="4"/>
-    <col min="3" max="3" width="50.83203125" customWidth="1"/>
+    <col min="3" max="3" width="67" customWidth="1"/>
     <col min="4" max="4" width="34.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
@@ -1238,7 +1292,7 @@
         <v>52</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>53</v>
@@ -1247,7 +1301,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1258,13 +1312,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="48">
+    <row r="3" spans="1:7" ht="48">
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -1272,13 +1326,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -1286,41 +1340,41 @@
         <v>42</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>81</v>
+      <c r="D5" s="18">
+        <v>2016</v>
       </c>
       <c r="E5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="B6" s="4">
         <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>82</v>
+      <c r="D6" s="18">
+        <v>2016</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1331,16 +1385,19 @@
         <v>7</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>102</v>
+      </c>
+      <c r="G7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -1348,33 +1405,33 @@
         <v>35</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="B9" s="4">
         <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>83</v>
+      <c r="D9" s="17">
+        <v>9</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="B10" s="4">
         <v>9</v>
       </c>
@@ -1382,16 +1439,16 @@
         <v>9</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="B11" s="4">
         <v>10</v>
       </c>
@@ -1399,33 +1456,33 @@
         <v>10</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="B12" s="4">
         <v>11</v>
       </c>
       <c r="C12" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>84</v>
+      <c r="D12" s="17">
+        <v>4</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="B13" s="4">
         <v>12</v>
       </c>
@@ -1433,16 +1490,16 @@
         <v>11</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="B14" s="4">
         <v>13</v>
       </c>
@@ -1450,47 +1507,50 @@
         <v>12</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="B15" s="4">
         <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>84</v>
+      <c r="D15" s="17">
+        <v>0</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>103</v>
+      </c>
+      <c r="G15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="B16" s="4">
         <v>15</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>85</v>
+      <c r="D16" s="17">
+        <v>28</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1504,13 +1564,13 @@
         <v>16</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1520,14 +1580,14 @@
       <c r="C18" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>86</v>
+      <c r="D18" s="17">
+        <v>42</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1544,7 +1604,7 @@
         <v>25</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1555,13 +1615,13 @@
         <v>17</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1572,13 +1632,13 @@
         <v>37</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1589,13 +1649,13 @@
         <v>18</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1605,14 +1665,14 @@
       <c r="C23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>111</v>
+      <c r="D23" s="20">
+        <v>6</v>
       </c>
       <c r="E23" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>154</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1622,14 +1682,14 @@
       <c r="C24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="20" t="s">
-        <v>112</v>
+      <c r="D24" s="20">
+        <v>12</v>
       </c>
       <c r="E24" t="s">
         <v>25</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>154</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1643,13 +1703,13 @@
         <v>38</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="E25" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1660,13 +1720,13 @@
         <v>39</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="E26" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1676,14 +1736,14 @@
       <c r="C27" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="20" t="s">
-        <v>87</v>
+      <c r="D27" s="20">
+        <v>2</v>
       </c>
       <c r="E27" t="s">
         <v>40</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>58</v>
@@ -1696,14 +1756,14 @@
       <c r="C28" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="20" t="s">
-        <v>88</v>
+      <c r="D28" s="20">
+        <v>4</v>
       </c>
       <c r="E28" t="s">
         <v>40</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -1715,13 +1775,13 @@
         <v>41</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="E29" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1732,13 +1792,13 @@
         <v>44</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="E30" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1748,14 +1808,14 @@
       <c r="C31" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="20" t="s">
-        <v>92</v>
+      <c r="D31" s="20">
+        <v>140</v>
       </c>
       <c r="E31" t="s">
         <v>25</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="G31" t="s">
         <v>23</v>
@@ -1768,14 +1828,14 @@
       <c r="C32" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>93</v>
+      <c r="D32" s="20">
+        <v>2</v>
       </c>
       <c r="E32" t="s">
         <v>27</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="G32" t="s">
         <v>24</v>
@@ -1789,16 +1849,16 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="48">
@@ -1806,16 +1866,16 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1826,13 +1886,13 @@
         <v>29</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="E35" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1842,14 +1902,14 @@
       <c r="C36" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="20" t="s">
-        <v>97</v>
+      <c r="D36" s="20">
+        <v>2</v>
       </c>
       <c r="E36" t="s">
         <v>25</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1860,13 +1920,13 @@
         <v>56</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
       <c r="G37" t="s">
         <v>46</v>
@@ -1879,14 +1939,14 @@
       <c r="C38" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="20" t="s">
-        <v>96</v>
+      <c r="D38" s="20">
+        <v>0</v>
       </c>
       <c r="E38" t="s">
         <v>25</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1897,13 +1957,13 @@
         <v>33</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="E39" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
       <c r="G39" t="s">
         <v>47</v>
@@ -1917,13 +1977,13 @@
         <v>34</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="E40" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="G40" t="s">
         <v>47</v>
@@ -1941,7 +2001,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F12"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1965,10 +2025,10 @@
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
@@ -1995,11 +2055,21 @@
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2018</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
@@ -2103,12 +2173,12 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F12"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -2127,10 +2197,10 @@
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
@@ -2157,21 +2227,41 @@
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="B3" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="27">
+        <v>3</v>
+      </c>
+      <c r="E3" s="27">
+        <v>3</v>
+      </c>
+      <c r="F3" s="27">
+        <v>2018</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="B4" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="27">
+        <v>3</v>
+      </c>
+      <c r="E4" s="27">
+        <v>3</v>
+      </c>
+      <c r="F4" s="27">
+        <v>2018</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
@@ -2265,7 +2355,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="I32" activeCellId="1" sqref="J23 I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2279,29 +2369,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickTop="1" thickBot="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="26" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12" ht="17" thickTop="1" thickBot="1">
-      <c r="A2" s="25"/>
+      <c r="A2" s="28"/>
       <c r="B2" s="11" t="s">
         <v>59</v>
       </c>
@@ -2318,10 +2408,10 @@
         <v>60</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>59</v>
@@ -2330,10 +2420,10 @@
         <v>60</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" thickTop="1" thickBot="1">
@@ -2341,19 +2431,19 @@
         <v>65</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="D3" s="9">
         <v>2017</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="G3" s="9">
         <v>2012</v>
@@ -2559,29 +2649,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickTop="1" thickBot="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="26" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12" ht="17" thickTop="1" thickBot="1">
-      <c r="A2" s="25"/>
+      <c r="A2" s="28"/>
       <c r="B2" s="11" t="s">
         <v>59</v>
       </c>
@@ -2598,10 +2688,10 @@
         <v>60</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>59</v>
@@ -2610,10 +2700,10 @@
         <v>60</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" thickTop="1" thickBot="1">
@@ -2630,10 +2720,10 @@
         <v>2017</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="G3" s="9">
         <v>2012</v>
@@ -2849,10 +2939,10 @@
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
@@ -2987,12 +3077,12 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3009,7 +3099,7 @@
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3034,16 +3124,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
       </c>
       <c r="E3" s="5">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3051,16 +3141,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3068,53 +3158,85 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="5">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2016</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2016</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2016</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
         <v>7</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2016</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A10" s="15">
@@ -3156,12 +3278,12 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3178,7 +3300,7 @@
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3203,16 +3325,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D3" s="5">
         <v>3</v>
       </c>
       <c r="E3" s="5">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3220,16 +3342,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D4" s="5">
         <v>3</v>
       </c>
       <c r="E4" s="5">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3237,16 +3359,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D5" s="5">
         <v>3</v>
       </c>
       <c r="E5" s="5">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3254,26 +3376,34 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D6" s="5">
         <v>3</v>
       </c>
       <c r="E6" s="5">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2016</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
@@ -3331,14 +3461,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E12"/>
+    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3355,7 +3485,7 @@
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3383,13 +3513,13 @@
         <v>135</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="D3" s="23">
         <v>3</v>
       </c>
       <c r="E3" s="5">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3397,16 +3527,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D4" s="23">
         <v>3</v>
       </c>
       <c r="E4" s="5">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3414,16 +3544,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D5" s="23">
         <v>3</v>
       </c>
       <c r="E5" s="5">
-        <v>2021</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3501,12 +3631,12 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3523,7 +3653,7 @@
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3547,79 +3677,103 @@
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="22">
+      <c r="D3" s="23">
         <v>4</v>
       </c>
-      <c r="E3" s="5">
-        <v>2021</v>
+      <c r="E3" s="25">
+        <v>2016</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="D4" s="22">
+      <c r="D4" s="23">
         <v>4</v>
       </c>
-      <c r="E4" s="5">
-        <v>2021</v>
+      <c r="E4" s="25">
+        <v>2016</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="22">
+      <c r="D5" s="23">
         <v>4</v>
       </c>
-      <c r="E5" s="5">
-        <v>2021</v>
+      <c r="E5" s="25">
+        <v>2016</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="23">
+        <v>4</v>
+      </c>
+      <c r="E6" s="25">
+        <v>2016</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="B7" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="23">
+        <v>4</v>
+      </c>
+      <c r="E7" s="25">
+        <v>2016</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A8" s="15">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="B8" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="23">
+        <v>4</v>
+      </c>
+      <c r="E8" s="25">
+        <v>2016</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A9" s="15">
@@ -3669,7 +3823,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3691,7 +3845,7 @@
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3715,35 +3869,19 @@
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="22">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5">
-        <v>2021</v>
-      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="22">
-        <v>3</v>
-      </c>
-      <c r="E4" s="5">
-        <v>2021</v>
-      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
@@ -3830,7 +3968,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3852,7 +3990,7 @@
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1">
@@ -3876,35 +4014,19 @@
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="D3" s="22">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5">
-        <v>2021</v>
-      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="D4" s="22">
-        <v>3</v>
-      </c>
-      <c r="E4" s="5">
-        <v>2021</v>
-      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
@@ -3991,12 +4113,12 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
   </cols>
@@ -4015,10 +4137,10 @@
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
@@ -4045,41 +4167,81 @@
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2016</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2016</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2016</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2016</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A7" s="15">
@@ -4153,7 +4315,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4177,10 +4339,10 @@
         <v>25</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" thickBot="1">
@@ -4207,11 +4369,21 @@
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2016</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="17" thickTop="1" thickBot="1">
       <c r="A4" s="15">

</xml_diff>